<commit_message>
updates png's and file locations
</commit_message>
<xml_diff>
--- a/assign01/data/csv/analysis/charts.xlsx
+++ b/assign01/data/csv/analysis/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timgao/Library/Mobile Documents/com~apple~CloudDocs/NEU/6650/cs6650-fa21/assign01/data/csv/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5179DF8-25A7-7346-88A0-4D129BC34B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2329187-6469-E240-A70E-2A9D65516E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24060" windowHeight="15500" activeTab="1" xr2:uid="{3FD36725-F4FF-A843-95BB-9D9E709BEBCC}"/>
   </bookViews>
@@ -16,10 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$B$10:$E$10</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$B$4:$E$4</definedName>
-  </definedNames>
   <calcPr calcId="181029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>threads</t>
   </si>
@@ -72,6 +68,9 @@
   </si>
   <si>
     <t>part2</t>
+  </si>
+  <si>
+    <t>trend</t>
   </si>
 </sst>
 </file>
@@ -127,406 +126,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Wall Time by Threads (ms by part)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Part1</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$E$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>390486</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>213692</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>124623</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>79733</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0817-B146-A6A1-A3FC99166B00}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Part2</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$10:$E$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>399636</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>206530</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>114642</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>72433</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0817-B146-A6A1-A3FC99166B00}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1436595519"/>
-        <c:axId val="1436597167"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1436595519"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1436597167"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1436597167"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1436595519"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -946,7 +545,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1362,7 +961,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1568,6 +1167,49 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-96C9-BF41-9C12-CD7A1AE17775}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Theoretical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>427.99680000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>855.99360000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1711.9872</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3423.9744000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8DB2-B04E-AC7B-2DF435D8B44E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1767,7 +1409,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2327,46 +1969,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4379,551 +3981,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C772090D-9EAC-AB44-B4D2-E41DFEC4AB2C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5377,17 +4435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62F7821-884C-2042-99EB-A5725B322043}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -5604,9 +4663,47 @@
         <v>437</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>420563.25</v>
+      </c>
+      <c r="C18">
+        <v>210281.625</v>
+      </c>
+      <c r="D18">
+        <v>105140.8125</v>
+      </c>
+      <c r="E18">
+        <v>52570.40625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>427.99680000000001</v>
+      </c>
+      <c r="C19">
+        <v>855.99360000000001</v>
+      </c>
+      <c r="D19">
+        <v>1711.9872</v>
+      </c>
+      <c r="E19">
+        <v>3423.9744000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5614,8 +4711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5ACB05-E5EC-C042-BE77-D0BFD637F442}">
   <dimension ref="L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="L77" sqref="L77"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="M76" sqref="M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates charts.xlsx with latest charts
</commit_message>
<xml_diff>
--- a/assign01/data/csv/analysis/charts.xlsx
+++ b/assign01/data/csv/analysis/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timgao/Library/Mobile Documents/com~apple~CloudDocs/NEU/6650/cs6650-fa21/assign01/data/csv/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2329187-6469-E240-A70E-2A9D65516E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5576527C-5350-5446-A9F6-E499F0E00F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24060" windowHeight="15500" activeTab="1" xr2:uid="{3FD36725-F4FF-A843-95BB-9D9E709BEBCC}"/>
   </bookViews>
@@ -1610,6 +1610,49 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8A05-4E47-828C-22C732040F31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Theoretical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>420563.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210281.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>105140.8125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52570.40625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A82F-B440-B2CC-C28EAFD01BE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4711,8 +4754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5ACB05-E5EC-C042-BE77-D0BFD637F442}">
   <dimension ref="L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates README.md with latest data
</commit_message>
<xml_diff>
--- a/assign01/data/csv/analysis/charts.xlsx
+++ b/assign01/data/csv/analysis/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timgao/Library/Mobile Documents/com~apple~CloudDocs/NEU/6650/cs6650-fa21/assign01/data/csv/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4035A32-2847-0542-81D3-05D7E641B54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D01CBA-FFD2-F54D-B592-96FBA32F81A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24220" windowHeight="15500" xr2:uid="{3FD36725-F4FF-A843-95BB-9D9E709BEBCC}"/>
   </bookViews>
@@ -8513,7 +8513,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A7" sqref="A7:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>